<commit_message>
refactoring, tried a module, undid it, then switched from eventReactive to using reactiveValues.
</commit_message>
<xml_diff>
--- a/tests/testthat/data/test.xlsx
+++ b/tests/testthat/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -68,6 +68,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,29 +154,182 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -200,7 +354,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -241,7 +395,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -282,7 +436,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -319,196 +473,196 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>2001</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>2001</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="0" t="n">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>2001</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>2001</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>2002</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>2002</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>2002</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>2002</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>2003</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="0" t="n">
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>2003</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="0" t="n">
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>2003</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="0" t="n">
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>2003</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="0" t="n">
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>24</v>
       </c>
     </row>

</xml_diff>